<commit_message>
Atlas2 catalog and star classes: all test OK
</commit_message>
<xml_diff>
--- a/AstroLib Master Layout.xlsx
+++ b/AstroLib Master Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevCS\AstroLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0810E10-98A6-4134-8047-741CBA504B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D700E2-45D9-4237-BFE3-84F367351D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20655" yWindow="510" windowWidth="17280" windowHeight="17565" activeTab="1" xr2:uid="{F0A37D56-3F1F-4302-A6DD-74EE141EC825}"/>
+    <workbookView xWindow="-19275" yWindow="375" windowWidth="17580" windowHeight="16395" activeTab="3" xr2:uid="{F0A37D56-3F1F-4302-A6DD-74EE141EC825}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>namespace: AstroLib.Catalog</t>
   </si>
   <si>
-    <t>AtlasRefcat2</t>
-  </si>
-  <si>
     <t>read and handle ATLAS Refcat2 catalog comp stars as selected</t>
   </si>
   <si>
@@ -294,6 +291,9 @@
   </si>
   <si>
     <t>collection of numerical methods</t>
+  </si>
+  <si>
+    <t>Atlas2</t>
   </si>
 </sst>
 </file>
@@ -747,7 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDD1E6F-A5A1-4F40-9237-A9A7F097497B}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -760,7 +760,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,10 +847,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
         <v>82</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -914,7 +914,7 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -968,17 +968,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -986,10 +986,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62C00AE-012E-494E-A467-998BB0A0AD1A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1014,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,15 +1032,15 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,12 +1048,12 @@
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1078,17 +1078,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1096,28 +1096,28 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,17 +1125,17 @@
         <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1168,17 +1168,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,10 +1186,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1214,17 +1214,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,22 +1232,22 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1255,26 +1255,26 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
         <v>63</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doxygen adds; start on AstroLib.Observer
Doxygen adds; start on AstroLib.Observer
</commit_message>
<xml_diff>
--- a/AstroLib Master Layout.xlsx
+++ b/AstroLib Master Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevCS\AstroLib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D700E2-45D9-4237-BFE3-84F367351D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFF994A-FBB4-474C-907F-94014A1E4B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19275" yWindow="375" windowWidth="17580" windowHeight="16395" activeTab="3" xr2:uid="{F0A37D56-3F1F-4302-A6DD-74EE141EC825}"/>
+    <workbookView xWindow="-21675" yWindow="915" windowWidth="19515" windowHeight="16665" activeTab="6" xr2:uid="{F0A37D56-3F1F-4302-A6DD-74EE141EC825}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name=".Catalog" sheetId="3" r:id="rId4"/>
     <sheet name=".Image" sheetId="6" r:id="rId5"/>
     <sheet name=".IO" sheetId="4" r:id="rId6"/>
-    <sheet name=".Observing" sheetId="7" r:id="rId7"/>
+    <sheet name=".Observer" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="85">
   <si>
     <t>SUMMARY</t>
   </si>
@@ -212,9 +212,6 @@
     <t>hold several related MonoImage instances</t>
   </si>
   <si>
-    <t>namespace: AstroLib.Observing.Earth</t>
-  </si>
-  <si>
     <t>Site</t>
   </si>
   <si>
@@ -227,12 +224,6 @@
     <t>Camera</t>
   </si>
   <si>
-    <t>namespace: AstroLib.Observing.Equipment</t>
-  </si>
-  <si>
-    <t>Building</t>
-  </si>
-  <si>
     <t>dome or roof</t>
   </si>
   <si>
@@ -281,9 +272,6 @@
     <t>project: AstroLib.Image</t>
   </si>
   <si>
-    <t>project: AstroLib.Observing</t>
-  </si>
-  <si>
     <t>namespace: AstroLib.Core.Maths</t>
   </si>
   <si>
@@ -294,6 +282,21 @@
   </si>
   <si>
     <t>Atlas2</t>
+  </si>
+  <si>
+    <t>Earth site definition: relatively fixed</t>
+  </si>
+  <si>
+    <t>Earth site's atmosphere; may be variable</t>
+  </si>
+  <si>
+    <t>project: AstroLib.Observer</t>
+  </si>
+  <si>
+    <t>namespace: AstroLib.Observer</t>
+  </si>
+  <si>
+    <t>Shelter</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -406,6 +409,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -760,7 +766,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +845,7 @@
     </row>
     <row r="15" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,10 +853,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -914,7 +920,7 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,7 +928,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -968,17 +974,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -986,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -1001,7 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62C00AE-012E-494E-A467-998BB0A0AD1A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1014,7 +1020,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1032,10 +1038,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
@@ -1078,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1168,7 +1174,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1184,7 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1199,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CF2A04-7503-4D30-A20B-D116456C5BB1}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1214,17 +1220,17 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>44</v>
+      <c r="A2" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,49 +1238,45 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="D7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
         <v>60</v>
-      </c>
-      <c r="D12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>